<commit_message>
Update video capture code
</commit_message>
<xml_diff>
--- a/testfile.xlsx
+++ b/testfile.xlsx
@@ -375,27 +375,27 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>158</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -435,22 +435,22 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
@@ -460,7 +460,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">

</xml_diff>